<commit_message>
updated soccer_schema and added soccer.sql
</commit_message>
<xml_diff>
--- a/schema_design_exercise.xlsx
+++ b/schema_design_exercise.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
   <si>
     <t>DOCTORS</t>
   </si>
@@ -117,9 +117,6 @@
     <t>"Robert Brown saw Mary Pepper on 8/25/2021 and found COVID"</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>visit_date</t>
   </si>
   <si>
@@ -189,15 +186,6 @@
     <t>team_id</t>
   </si>
   <si>
-    <t>GAME</t>
-  </si>
-  <si>
-    <t>team1</t>
-  </si>
-  <si>
-    <t>team2</t>
-  </si>
-  <si>
     <t>REFEREES</t>
   </si>
   <si>
@@ -213,21 +201,12 @@
     <t>SEASONS</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
     <t>game_id</t>
   </si>
   <si>
     <t>player_id</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>season_id</t>
   </si>
   <si>
@@ -238,6 +217,138 @@
   </si>
   <si>
     <t>PLAYER-TEAM</t>
+  </si>
+  <si>
+    <t>RUS</t>
+  </si>
+  <si>
+    <t>UKR</t>
+  </si>
+  <si>
+    <t>SPA</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>Torpeda</t>
+  </si>
+  <si>
+    <t>Dinamo</t>
+  </si>
+  <si>
+    <t>Barselona</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>player1</t>
+  </si>
+  <si>
+    <t>player2</t>
+  </si>
+  <si>
+    <t>player3</t>
+  </si>
+  <si>
+    <t>player4</t>
+  </si>
+  <si>
+    <t>referee1</t>
+  </si>
+  <si>
+    <t>referee2</t>
+  </si>
+  <si>
+    <t>referee3</t>
+  </si>
+  <si>
+    <t>referee4</t>
+  </si>
+  <si>
+    <t>player5</t>
+  </si>
+  <si>
+    <t>player6</t>
+  </si>
+  <si>
+    <t>player7</t>
+  </si>
+  <si>
+    <t>player8</t>
+  </si>
+  <si>
+    <t>player9</t>
+  </si>
+  <si>
+    <t>player10</t>
+  </si>
+  <si>
+    <t>player11</t>
+  </si>
+  <si>
+    <t>player12</t>
+  </si>
+  <si>
+    <t>player13</t>
+  </si>
+  <si>
+    <t>player14</t>
+  </si>
+  <si>
+    <t>player15</t>
+  </si>
+  <si>
+    <t>player16</t>
+  </si>
+  <si>
+    <t>game1: score1 =1, score2=1</t>
+  </si>
+  <si>
+    <t>game2: score1=2, score2=0</t>
+  </si>
+  <si>
+    <t>game3: score1=1, score2=3</t>
+  </si>
+  <si>
+    <t>RUS/UKR</t>
+  </si>
+  <si>
+    <t>RUS/SPA</t>
+  </si>
+  <si>
+    <t>RUS/ITA</t>
+  </si>
+  <si>
+    <t>start_dat</t>
+  </si>
+  <si>
+    <t>end_dat</t>
+  </si>
+  <si>
+    <t>game_date</t>
+  </si>
+  <si>
+    <t>GAMES</t>
+  </si>
+  <si>
+    <t>team1_id</t>
+  </si>
+  <si>
+    <t>team2_id</t>
+  </si>
+  <si>
+    <t>time_scored</t>
+  </si>
+  <si>
+    <t>score_1</t>
+  </si>
+  <si>
+    <t>score_2</t>
+  </si>
+  <si>
+    <t>ranking</t>
   </si>
 </sst>
 </file>
@@ -405,9 +516,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -464,7 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,6 +582,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,49 +642,13 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -561,14 +675,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -889,168 +1001,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="D1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="36"/>
-      <c r="H1" s="37" t="s">
+      <c r="B1" s="47"/>
+      <c r="D1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="49"/>
+      <c r="H1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="38"/>
+      <c r="I1" s="51"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="17">
-        <v>1</v>
-      </c>
-      <c r="I4" s="19" t="s">
+      <c r="H4" s="16">
+        <v>1</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11">
-        <v>2</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17">
-        <v>2</v>
-      </c>
-      <c r="I5" s="19" t="s">
+      <c r="H5" s="16">
+        <v>2</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="11">
-        <v>3</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="17">
-        <v>3</v>
-      </c>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="16">
+        <v>3</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>4</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>34</v>
+      <c r="D11" s="25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <v>1</v>
-      </c>
-      <c r="B13" s="25">
-        <v>1</v>
-      </c>
-      <c r="C13" s="25">
-        <v>1</v>
-      </c>
-      <c r="D13" s="32">
+      <c r="A13" s="24">
+        <v>1</v>
+      </c>
+      <c r="B13" s="24">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1</v>
+      </c>
+      <c r="D13" s="30">
         <v>44433</v>
       </c>
       <c r="F13" t="s">
@@ -1058,16 +1170,16 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
-        <v>2</v>
-      </c>
-      <c r="B14" s="25">
-        <v>1</v>
-      </c>
-      <c r="C14" s="25">
-        <v>2</v>
-      </c>
-      <c r="D14" s="32">
+      <c r="A14" s="24">
+        <v>2</v>
+      </c>
+      <c r="B14" s="24">
+        <v>1</v>
+      </c>
+      <c r="C14" s="24">
+        <v>2</v>
+      </c>
+      <c r="D14" s="30">
         <v>44433</v>
       </c>
       <c r="F14" t="s">
@@ -1075,16 +1187,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
-        <v>3</v>
-      </c>
-      <c r="B15" s="25">
-        <v>2</v>
-      </c>
-      <c r="C15" s="25">
-        <v>1</v>
-      </c>
-      <c r="D15" s="32">
+      <c r="A15" s="24">
+        <v>3</v>
+      </c>
+      <c r="B15" s="24">
+        <v>2</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30">
         <v>44433</v>
       </c>
       <c r="F15" t="s">
@@ -1092,16 +1204,16 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
+      <c r="A16" s="24">
         <v>4</v>
       </c>
-      <c r="B16" s="25">
-        <v>3</v>
-      </c>
-      <c r="C16" s="25">
-        <v>1</v>
-      </c>
-      <c r="D16" s="32">
+      <c r="B16" s="24">
+        <v>3</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1</v>
+      </c>
+      <c r="D16" s="30">
         <v>44433</v>
       </c>
       <c r="F16" t="s">
@@ -1109,32 +1221,32 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="56"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>35</v>
+      <c r="B20" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="31">
-        <v>1</v>
-      </c>
-      <c r="B22" s="31">
+      <c r="A22" s="29">
+        <v>1</v>
+      </c>
+      <c r="B22" s="29">
         <v>1</v>
       </c>
       <c r="D22" t="s">
@@ -1142,10 +1254,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="31">
-        <v>1</v>
-      </c>
-      <c r="B23" s="31">
+      <c r="A23" s="29">
+        <v>1</v>
+      </c>
+      <c r="B23" s="29">
         <v>3</v>
       </c>
       <c r="D23" t="s">
@@ -1153,10 +1265,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="31">
-        <v>2</v>
-      </c>
-      <c r="B24" s="31">
+      <c r="A24" s="29">
+        <v>2</v>
+      </c>
+      <c r="B24" s="29">
         <v>2</v>
       </c>
       <c r="D24" t="s">
@@ -1164,10 +1276,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="31">
-        <v>3</v>
-      </c>
-      <c r="B25" s="31">
+      <c r="A25" s="29">
+        <v>3</v>
+      </c>
+      <c r="B25" s="29">
         <v>1</v>
       </c>
       <c r="D25" t="s">
@@ -1207,179 +1319,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="F1" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="J1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="F1" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="J1" s="16" t="s">
+      <c r="F2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="16"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="B7" s="20"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B9" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="21"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1388,276 +1500,790 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="4" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="34">
+        <v>1</v>
+      </c>
+      <c r="B4" s="68">
+        <v>44378</v>
+      </c>
+      <c r="C4" s="68">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="64"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="32"/>
+      <c r="J6" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="M6" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="41"/>
+      <c r="O6" s="42"/>
+      <c r="Q6" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" s="44"/>
+      <c r="S6" s="45"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="S7" s="37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="J8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="K8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="32">
+        <v>1</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="J9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="70">
+        <v>1</v>
+      </c>
+      <c r="N9" s="70">
+        <v>1</v>
+      </c>
+      <c r="O9" s="70">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="38">
+        <v>1</v>
+      </c>
+      <c r="R9" s="38">
+        <v>1</v>
+      </c>
+      <c r="S9" s="38">
+        <v>20</v>
+      </c>
+      <c r="U9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="32">
+        <v>2</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="J10" s="13">
+        <v>2</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="70">
+        <v>2</v>
+      </c>
+      <c r="N10" s="70">
+        <v>1</v>
+      </c>
+      <c r="O10" s="70">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="38">
+        <v>1</v>
+      </c>
+      <c r="R10" s="38">
+        <v>5</v>
+      </c>
+      <c r="S10" s="38">
+        <v>40</v>
+      </c>
+      <c r="U10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="32">
+        <v>3</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="J11" s="13">
+        <v>3</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="70">
+        <v>3</v>
+      </c>
+      <c r="N11" s="70">
+        <v>1</v>
+      </c>
+      <c r="O11" s="70">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="38">
+        <v>2</v>
+      </c>
+      <c r="R11" s="38">
+        <v>1</v>
+      </c>
+      <c r="S11" s="38">
+        <v>2</v>
+      </c>
+      <c r="U11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="32">
+        <v>4</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="J12" s="13">
+        <v>4</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="70">
+        <v>4</v>
+      </c>
+      <c r="N12" s="70">
+        <v>1</v>
+      </c>
+      <c r="O12" s="70">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="38">
+        <v>2</v>
+      </c>
+      <c r="R12" s="38">
+        <v>2</v>
+      </c>
+      <c r="S12" s="38">
+        <v>47</v>
+      </c>
+      <c r="U12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J13" s="13">
+        <v>5</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" s="70">
+        <v>5</v>
+      </c>
+      <c r="N13" s="70">
+        <v>1</v>
+      </c>
+      <c r="O13" s="70">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="38">
+        <v>3</v>
+      </c>
+      <c r="R13" s="38">
+        <v>3</v>
+      </c>
+      <c r="S13" s="38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="62"/>
+      <c r="J14" s="13">
+        <v>6</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M14" s="70">
+        <v>6</v>
+      </c>
+      <c r="N14" s="70">
+        <v>1</v>
+      </c>
+      <c r="O14" s="70">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="38">
+        <v>3</v>
+      </c>
+      <c r="R14" s="38">
+        <v>15</v>
+      </c>
+      <c r="S14" s="38">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="13">
+        <v>7</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M15" s="70">
+        <v>7</v>
+      </c>
+      <c r="N15" s="70">
+        <v>1</v>
+      </c>
+      <c r="O15" s="70">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="38">
+        <v>3</v>
+      </c>
+      <c r="R15" s="38">
+        <v>15</v>
+      </c>
+      <c r="S15" s="38">
+        <v>30</v>
+      </c>
+      <c r="U15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="66"/>
-      <c r="E6" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="36"/>
-      <c r="J6" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+      <c r="H16" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="13">
+        <v>8</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="M16" s="70">
+        <v>8</v>
+      </c>
+      <c r="N16" s="70">
+        <v>1</v>
+      </c>
+      <c r="O16" s="70">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="38">
+        <v>3</v>
+      </c>
+      <c r="R16" s="38">
+        <v>16</v>
+      </c>
+      <c r="S16" s="38">
+        <v>42</v>
+      </c>
+      <c r="U16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="28">
+        <v>1</v>
+      </c>
+      <c r="B17" s="28">
+        <v>1</v>
+      </c>
+      <c r="C17" s="28">
+        <v>2</v>
+      </c>
+      <c r="D17" s="28">
+        <v>1</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="69">
+        <v>44379</v>
+      </c>
+      <c r="H17" s="28">
+        <v>1</v>
+      </c>
+      <c r="J17" s="13">
+        <v>9</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" s="70">
+        <v>9</v>
+      </c>
+      <c r="N17" s="70">
+        <v>1</v>
+      </c>
+      <c r="O17" s="70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="28">
+        <v>2</v>
+      </c>
+      <c r="B18" s="28">
+        <v>1</v>
+      </c>
+      <c r="C18" s="28">
+        <v>3</v>
+      </c>
+      <c r="D18" s="28">
+        <v>2</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="69">
+        <v>44381</v>
+      </c>
+      <c r="H18" s="28">
+        <v>1</v>
+      </c>
+      <c r="J18" s="13">
+        <v>10</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="70">
+        <v>10</v>
+      </c>
+      <c r="N18" s="70">
+        <v>1</v>
+      </c>
+      <c r="O18" s="70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="28">
+        <v>3</v>
+      </c>
+      <c r="B19" s="28">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28">
+        <v>4</v>
+      </c>
+      <c r="D19" s="28">
+        <v>1</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="69">
+        <v>44383</v>
+      </c>
+      <c r="H19" s="28">
+        <v>1</v>
+      </c>
+      <c r="J19" s="13">
         <v>11</v>
       </c>
-      <c r="B8" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="45" t="s">
+      <c r="K19" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="M19" s="70">
+        <v>11</v>
+      </c>
+      <c r="N19" s="70">
+        <v>1</v>
+      </c>
+      <c r="O19" s="70">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" s="67"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="28">
+        <v>4</v>
+      </c>
+      <c r="B20" s="28">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28">
+        <v>3</v>
+      </c>
+      <c r="D20" s="28">
+        <v>3</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="69">
+        <v>44385</v>
+      </c>
+      <c r="H20" s="28">
+        <v>1</v>
+      </c>
+      <c r="J20" s="13">
+        <v>12</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="70">
+        <v>12</v>
+      </c>
+      <c r="N20" s="70">
+        <v>1</v>
+      </c>
+      <c r="O20" s="70">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="28">
+        <v>5</v>
+      </c>
+      <c r="B21" s="28">
+        <v>2</v>
+      </c>
+      <c r="C21" s="28">
+        <v>4</v>
+      </c>
+      <c r="D21" s="28">
+        <v>4</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="69">
+        <v>44387</v>
+      </c>
+      <c r="H21" s="28">
+        <v>1</v>
+      </c>
+      <c r="J21" s="13">
+        <v>13</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="M21" s="70">
+        <v>13</v>
+      </c>
+      <c r="N21" s="70">
+        <v>1</v>
+      </c>
+      <c r="O21" s="70">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="R21" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="63"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="E18" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="28">
+        <v>6</v>
+      </c>
+      <c r="B22" s="28">
+        <v>3</v>
+      </c>
+      <c r="C22" s="28">
+        <v>4</v>
+      </c>
+      <c r="D22" s="28">
+        <v>4</v>
+      </c>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="69">
+        <v>44389</v>
+      </c>
+      <c r="H22" s="28">
+        <v>1</v>
+      </c>
+      <c r="J22" s="13">
+        <v>14</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="70">
+        <v>14</v>
+      </c>
+      <c r="N22" s="70">
+        <v>1</v>
+      </c>
+      <c r="O22" s="70">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>1</v>
+      </c>
+      <c r="R22" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J23" s="13">
+        <v>15</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="M23" s="70">
+        <v>15</v>
+      </c>
+      <c r="N23" s="70">
+        <v>1</v>
+      </c>
+      <c r="O23" s="70">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="18">
+        <v>2</v>
+      </c>
+      <c r="R23" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J24" s="13">
+        <v>16</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M24" s="70">
+        <v>16</v>
+      </c>
+      <c r="N24" s="70">
+        <v>1</v>
+      </c>
+      <c r="O24" s="70">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="18">
+        <v>3</v>
+      </c>
+      <c r="R24" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q25" s="18">
+        <v>4</v>
+      </c>
+      <c r="R25" s="18" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added ranking calculation to soccer.sql
</commit_message>
<xml_diff>
--- a/schema_design_exercise.xlsx
+++ b/schema_design_exercise.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Craigslist" sheetId="2" r:id="rId2"/>
     <sheet name="Soccer League" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="118">
   <si>
     <t>DOCTORS</t>
   </si>
@@ -150,9 +150,6 @@
     <t>POSTS</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>location_id</t>
   </si>
   <si>
@@ -348,7 +345,31 @@
     <t>score_2</t>
   </si>
   <si>
-    <t>ranking</t>
+    <t>standing_1</t>
+  </si>
+  <si>
+    <t>standing_2</t>
+  </si>
+  <si>
+    <t>goals scored during the game by team1</t>
+  </si>
+  <si>
+    <t>goals scored during the game by team2</t>
+  </si>
+  <si>
+    <t>current game standing  (0- loss/1-"dead heat"/2-win) for team1</t>
+  </si>
+  <si>
+    <t>current game standing  (0- loss/1-"dead heat"/2-win) for team2</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>post_text</t>
   </si>
 </sst>
 </file>
@@ -516,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -621,6 +642,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -660,21 +687,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,6 +694,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,18 +1023,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="D1" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="49"/>
-      <c r="H1" s="50" t="s">
+      <c r="B1" s="49"/>
+      <c r="D1" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="51"/>
+      <c r="H1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="51"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -1117,12 +1139,12 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
@@ -1221,10 +1243,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="56"/>
+      <c r="B19" s="58"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
@@ -1304,7 +1326,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,7 +1379,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>11</v>
@@ -1399,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1434,22 +1456,22 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>46</v>
-      </c>
       <c r="G14" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1457,7 +1479,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
@@ -1500,40 +1522,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
     <col min="4" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" customWidth="1"/>
+    <col min="7" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="4.88671875" customWidth="1"/>
+    <col min="14" max="14" width="5.77734375" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>11</v>
       </c>
@@ -1544,387 +1572,391 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="34">
         <v>1</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="65">
         <v>44378</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="65">
         <v>44409</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="63" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="68"/>
+      <c r="L6" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="51"/>
+      <c r="O6" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="42"/>
+      <c r="S6" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" s="44"/>
+      <c r="U6" s="45"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="32"/>
-      <c r="J6" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="49"/>
-      <c r="M6" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="41"/>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="45"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>51</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="12" t="s">
+      <c r="D7" s="69"/>
+      <c r="L7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q7" s="27" t="s">
+      <c r="S7" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="R7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="S7" s="37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U7" s="37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="13" t="s">
+      <c r="D8" s="68"/>
+      <c r="L8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="O8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="34" t="s">
+      <c r="P8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="32" t="s">
+      <c r="Q8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="28" t="s">
+      <c r="S8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="T8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U8" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="32">
         <v>1</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="L9" s="13">
+        <v>1</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="O9" s="67">
+        <v>1</v>
+      </c>
+      <c r="P9" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="67">
+        <v>1</v>
+      </c>
+      <c r="S9" s="38">
+        <v>1</v>
+      </c>
+      <c r="T9" s="38">
+        <v>1</v>
+      </c>
+      <c r="U9" s="38">
+        <v>20</v>
+      </c>
+      <c r="W9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="32">
+        <v>2</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C10" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="J9" s="13">
-        <v>1</v>
-      </c>
-      <c r="K9" s="13" t="s">
+      <c r="D10" s="68"/>
+      <c r="L10" s="13">
+        <v>2</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="70">
-        <v>1</v>
-      </c>
-      <c r="N9" s="70">
-        <v>1</v>
-      </c>
-      <c r="O9" s="70">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="38">
-        <v>1</v>
-      </c>
-      <c r="R9" s="38">
-        <v>1</v>
-      </c>
-      <c r="S9" s="38">
-        <v>20</v>
-      </c>
-      <c r="U9" t="s">
+      <c r="O10" s="67">
+        <v>2</v>
+      </c>
+      <c r="P10" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="67">
+        <v>1</v>
+      </c>
+      <c r="S10" s="38">
+        <v>1</v>
+      </c>
+      <c r="T10" s="38">
+        <v>5</v>
+      </c>
+      <c r="U10" s="38">
+        <v>40</v>
+      </c>
+      <c r="W10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" s="32">
+        <v>3</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="68"/>
+      <c r="L11" s="13">
+        <v>3</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="67">
+        <v>3</v>
+      </c>
+      <c r="P11" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="67">
+        <v>1</v>
+      </c>
+      <c r="S11" s="38">
+        <v>2</v>
+      </c>
+      <c r="T11" s="38">
+        <v>1</v>
+      </c>
+      <c r="U11" s="38">
+        <v>2</v>
+      </c>
+      <c r="W11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="32">
-        <v>2</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="32"/>
-      <c r="J10" s="13">
-        <v>2</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M10" s="70">
-        <v>2</v>
-      </c>
-      <c r="N10" s="70">
-        <v>1</v>
-      </c>
-      <c r="O10" s="70">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="38">
-        <v>1</v>
-      </c>
-      <c r="R10" s="38">
-        <v>5</v>
-      </c>
-      <c r="S10" s="38">
-        <v>40</v>
-      </c>
-      <c r="U10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="32">
-        <v>3</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="32"/>
-      <c r="J11" s="13">
-        <v>3</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="M11" s="70">
-        <v>3</v>
-      </c>
-      <c r="N11" s="70">
-        <v>1</v>
-      </c>
-      <c r="O11" s="70">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="38">
-        <v>2</v>
-      </c>
-      <c r="R11" s="38">
-        <v>1</v>
-      </c>
-      <c r="S11" s="38">
-        <v>2</v>
-      </c>
-      <c r="U11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
         <v>4</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="J12" s="13">
+        <v>73</v>
+      </c>
+      <c r="D12" s="68"/>
+      <c r="L12" s="13">
         <v>4</v>
       </c>
-      <c r="K12" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" s="70">
+      <c r="M12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" s="67">
         <v>4</v>
       </c>
-      <c r="N12" s="70">
-        <v>1</v>
-      </c>
-      <c r="O12" s="70">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="38">
-        <v>2</v>
-      </c>
-      <c r="R12" s="38">
-        <v>2</v>
+      <c r="P12" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="67">
+        <v>1</v>
       </c>
       <c r="S12" s="38">
+        <v>2</v>
+      </c>
+      <c r="T12" s="38">
+        <v>2</v>
+      </c>
+      <c r="U12" s="38">
         <v>47</v>
       </c>
-      <c r="U12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J13" s="13">
+      <c r="W12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="L13" s="13">
         <v>5</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="M13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="O13" s="67">
+        <v>5</v>
+      </c>
+      <c r="P13" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="67">
+        <v>2</v>
+      </c>
+      <c r="S13" s="38">
+        <v>3</v>
+      </c>
+      <c r="T13" s="38">
+        <v>3</v>
+      </c>
+      <c r="U13" s="38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="64"/>
+      <c r="L14" s="13">
+        <v>6</v>
+      </c>
+      <c r="M14" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="M13" s="70">
-        <v>5</v>
-      </c>
-      <c r="N13" s="70">
-        <v>1</v>
-      </c>
-      <c r="O13" s="70">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="38">
-        <v>3</v>
-      </c>
-      <c r="R13" s="38">
-        <v>3</v>
-      </c>
-      <c r="S13" s="38">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="60" t="s">
+      <c r="O14" s="67">
+        <v>6</v>
+      </c>
+      <c r="P14" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="67">
+        <v>2</v>
+      </c>
+      <c r="S14" s="38">
+        <v>3</v>
+      </c>
+      <c r="T14" s="38">
+        <v>15</v>
+      </c>
+      <c r="U14" s="38">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="62"/>
-      <c r="J14" s="13">
-        <v>6</v>
-      </c>
-      <c r="K14" s="13" t="s">
+      <c r="C15" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" s="13">
+        <v>7</v>
+      </c>
+      <c r="M15" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M14" s="70">
-        <v>6</v>
-      </c>
-      <c r="N14" s="70">
-        <v>1</v>
-      </c>
-      <c r="O14" s="70">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="38">
-        <v>3</v>
-      </c>
-      <c r="R14" s="38">
+      <c r="O15" s="67">
+        <v>7</v>
+      </c>
+      <c r="P15" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="67">
+        <v>2</v>
+      </c>
+      <c r="S15" s="38">
+        <v>3</v>
+      </c>
+      <c r="T15" s="38">
         <v>15</v>
       </c>
-      <c r="S14" s="38">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="13">
-        <v>7</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M15" s="70">
-        <v>7</v>
-      </c>
-      <c r="N15" s="70">
-        <v>1</v>
-      </c>
-      <c r="O15" s="70">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="38">
-        <v>3</v>
-      </c>
-      <c r="R15" s="38">
-        <v>15</v>
-      </c>
-      <c r="S15" s="38">
+      <c r="U15" s="38">
         <v>30</v>
       </c>
-      <c r="U15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="W15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>11</v>
       </c>
@@ -1938,46 +1970,52 @@
         <v>12</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="J16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="13">
+      <c r="L16" s="13">
         <v>8</v>
       </c>
-      <c r="K16" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="M16" s="70">
+      <c r="M16" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" s="67">
         <v>8</v>
       </c>
-      <c r="N16" s="70">
-        <v>1</v>
-      </c>
-      <c r="O16" s="70">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="38">
-        <v>3</v>
-      </c>
-      <c r="R16" s="38">
+      <c r="P16" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="67">
+        <v>2</v>
+      </c>
+      <c r="S16" s="38">
+        <v>3</v>
+      </c>
+      <c r="T16" s="38">
         <v>16</v>
       </c>
-      <c r="S16" s="38">
+      <c r="U16" s="38">
         <v>42</v>
       </c>
-      <c r="U16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="W16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>1</v>
       </c>
@@ -1992,29 +2030,31 @@
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
-      <c r="G17" s="69">
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="66">
         <v>44379</v>
       </c>
-      <c r="H17" s="28">
-        <v>1</v>
-      </c>
-      <c r="J17" s="13">
+      <c r="J17" s="28">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13">
         <v>9</v>
       </c>
-      <c r="K17" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="M17" s="70">
+      <c r="M17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="O17" s="67">
         <v>9</v>
       </c>
-      <c r="N17" s="70">
-        <v>1</v>
-      </c>
-      <c r="O17" s="70">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P17" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>2</v>
       </c>
@@ -2029,29 +2069,31 @@
       </c>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
-      <c r="G18" s="69">
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="66">
         <v>44381</v>
       </c>
-      <c r="H18" s="28">
-        <v>1</v>
-      </c>
-      <c r="J18" s="13">
+      <c r="J18" s="28">
+        <v>1</v>
+      </c>
+      <c r="L18" s="13">
         <v>10</v>
       </c>
-      <c r="K18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="M18" s="70">
+      <c r="M18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="O18" s="67">
         <v>10</v>
       </c>
-      <c r="N18" s="70">
-        <v>1</v>
-      </c>
-      <c r="O18" s="70">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P18" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
         <v>3</v>
       </c>
@@ -2066,33 +2108,35 @@
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
-      <c r="G19" s="69">
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="66">
         <v>44383</v>
       </c>
-      <c r="H19" s="28">
-        <v>1</v>
-      </c>
-      <c r="J19" s="13">
+      <c r="J19" s="28">
+        <v>1</v>
+      </c>
+      <c r="L19" s="13">
         <v>11</v>
       </c>
-      <c r="K19" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M19" s="70">
+      <c r="M19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="O19" s="67">
         <v>11</v>
       </c>
-      <c r="N19" s="70">
-        <v>1</v>
-      </c>
-      <c r="O19" s="70">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="R19" s="67"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P19" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="67">
+        <v>3</v>
+      </c>
+      <c r="S19" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="T19" s="47"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>4</v>
       </c>
@@ -2107,35 +2151,37 @@
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="69">
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="66">
         <v>44385</v>
       </c>
-      <c r="H20" s="28">
-        <v>1</v>
-      </c>
-      <c r="J20" s="13">
+      <c r="J20" s="28">
+        <v>1</v>
+      </c>
+      <c r="L20" s="13">
         <v>12</v>
       </c>
-      <c r="K20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="M20" s="70">
+      <c r="M20" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="O20" s="67">
         <v>12</v>
       </c>
-      <c r="N20" s="70">
-        <v>1</v>
-      </c>
-      <c r="O20" s="70">
-        <v>3</v>
-      </c>
-      <c r="Q20" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R20" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P20" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="67">
+        <v>3</v>
+      </c>
+      <c r="S20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T20" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>5</v>
       </c>
@@ -2150,35 +2196,37 @@
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
-      <c r="G21" s="69">
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="66">
         <v>44387</v>
       </c>
-      <c r="H21" s="28">
-        <v>1</v>
-      </c>
-      <c r="J21" s="13">
+      <c r="J21" s="28">
+        <v>1</v>
+      </c>
+      <c r="L21" s="13">
         <v>13</v>
       </c>
-      <c r="K21" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="M21" s="70">
+      <c r="M21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="O21" s="67">
         <v>13</v>
       </c>
-      <c r="N21" s="70">
-        <v>1</v>
-      </c>
-      <c r="O21" s="70">
+      <c r="P21" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="67">
         <v>4</v>
       </c>
-      <c r="Q21" s="18" t="s">
+      <c r="S21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="R21" s="18" t="s">
+      <c r="T21" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>6</v>
       </c>
@@ -2193,95 +2241,126 @@
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
-      <c r="G22" s="69">
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="66">
         <v>44389</v>
       </c>
-      <c r="H22" s="28">
-        <v>1</v>
-      </c>
-      <c r="J22" s="13">
+      <c r="J22" s="28">
+        <v>1</v>
+      </c>
+      <c r="L22" s="13">
         <v>14</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="M22" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O22" s="67">
+        <v>14</v>
+      </c>
+      <c r="P22" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="67">
+        <v>4</v>
+      </c>
+      <c r="S22" s="18">
+        <v>1</v>
+      </c>
+      <c r="T22" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L23" s="13">
+        <v>15</v>
+      </c>
+      <c r="M23" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="M22" s="70">
-        <v>14</v>
-      </c>
-      <c r="N22" s="70">
-        <v>1</v>
-      </c>
-      <c r="O22" s="70">
+      <c r="O23" s="67">
+        <v>15</v>
+      </c>
+      <c r="P23" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="67">
         <v>4</v>
       </c>
-      <c r="Q22" s="18">
-        <v>1</v>
-      </c>
-      <c r="R22" s="18" t="s">
+      <c r="S23" s="18">
+        <v>2</v>
+      </c>
+      <c r="T23" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J23" s="13">
-        <v>15</v>
-      </c>
-      <c r="K23" s="13" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L24" s="13">
+        <v>16</v>
+      </c>
+      <c r="M24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="M23" s="70">
-        <v>15</v>
-      </c>
-      <c r="N23" s="70">
-        <v>1</v>
-      </c>
-      <c r="O23" s="70">
+      <c r="O24" s="67">
+        <v>16</v>
+      </c>
+      <c r="P24" s="67">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="67">
         <v>4</v>
       </c>
-      <c r="Q23" s="18">
-        <v>2</v>
-      </c>
-      <c r="R23" s="18" t="s">
+      <c r="S24" s="18">
+        <v>3</v>
+      </c>
+      <c r="T24" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J24" s="13">
-        <v>16</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="M24" s="70">
-        <v>16</v>
-      </c>
-      <c r="N24" s="70">
-        <v>1</v>
-      </c>
-      <c r="O24" s="70">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="S25" s="18">
         <v>4</v>
       </c>
-      <c r="Q24" s="18">
-        <v>3</v>
-      </c>
-      <c r="R24" s="18" t="s">
+      <c r="T25" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="Q25" s="18">
-        <v>4</v>
-      </c>
-      <c r="R25" s="18" t="s">
-        <v>82</v>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="Q19:R19"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A14:J14"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>